<commit_message>
[ DSD-950 ] Set is_active to TRUE
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template.xlsx
+++ b/mosip_master/xlsx/template.xlsx
@@ -3904,11 +3904,11 @@
   </sheetPr>
   <dimension ref="A1:M467"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K468" activeCellId="0" sqref="K468"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.57"/>
@@ -22696,8 +22696,7 @@
       <c r="J465" s="0" t="s">
         <v>1040</v>
       </c>
-      <c r="K465" s="0" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="K465" s="2" t="b">
         <v>1</v>
       </c>
       <c r="L465" s="0" t="s">

</xml_diff>

<commit_message>
Revert "[ DSD-950 ] Set is_active to TRUE"
This reverts commit 7e64da1a96b88a332c892d305c0ac6ce864393e1.
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template.xlsx
+++ b/mosip_master/xlsx/template.xlsx
@@ -3904,11 +3904,11 @@
   </sheetPr>
   <dimension ref="A1:M467"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K468" activeCellId="0" sqref="K468"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.57"/>
@@ -22696,7 +22696,8 @@
       <c r="J465" s="0" t="s">
         <v>1040</v>
       </c>
-      <c r="K465" s="2" t="b">
+      <c r="K465" s="0" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="L465" s="0" t="s">

</xml_diff>

<commit_message>
[ DSD-950 ] Set is_active to \'TRUE\'
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template.xlsx
+++ b/mosip_master/xlsx/template.xlsx
@@ -82,7 +82,7 @@
     <t xml:space="preserve">auth-email-content</t>
   </si>
   <si>
-    <t xml:space="preserve">'true’</t>
+    <t xml:space="preserve">\'true\’</t>
   </si>
   <si>
     <t xml:space="preserve">superadmin</t>
@@ -1362,8 +1362,8 @@
   </sheetPr>
   <dimension ref="A1:M142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2:K142"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K142" activeCellId="0" sqref="K2:K142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>